<commit_message>
Amplify Shader Editor Problem with Sprite and UI Shader Types: Property (_MainTex) already exists. Use SetTexture instead
</commit_message>
<xml_diff>
--- a/Document/Excel/Buff.xlsx
+++ b/Document/Excel/Buff.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -114,6 +114,19 @@
   <si>
     <t>心跳检查时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
   </si>
 </sst>
 </file>
@@ -441,7 +454,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A5" sqref="A5:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -559,6 +572,9 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -567,6 +583,9 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -575,6 +594,9 @@
       <c r="E7">
         <v>0</v>
       </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -582,6 +604,9 @@
       </c>
       <c r="E8">
         <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>